<commit_message>
Code as Per Review 2
</commit_message>
<xml_diff>
--- a/datasets/EngineeringRanking.xlsx
+++ b/datasets/EngineeringRanking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\NIRFRankPredictor\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8A455191-FF23-463C-B5D1-F93F495F0424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05E96EF-A0E1-46C3-9C27-FD7EB15AF90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EngineeringRanking" sheetId="1" r:id="rId1"/>
@@ -2347,7 +2347,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2677,7 +2677,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -2864,6 +2864,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFC8CDC7"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFC8CDC7"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2909,7 +2920,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2928,6 +2939,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3277,24 +3294,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="AY2" sqref="AY2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="33.21875" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" hidden="1" customWidth="1"/>
     <col min="5" max="22" width="8.88671875" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="7.5546875" hidden="1" customWidth="1"/>
@@ -3303,10 +3320,20 @@
     <col min="26" max="29" width="8.88671875" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="1.6640625" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="31.33203125" hidden="1" customWidth="1"/>
-    <col min="32" max="38" width="8.88671875" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="8.6640625" hidden="1" customWidth="1"/>
-    <col min="40" max="46" width="8.88671875" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="9.21875" customWidth="1"/>
+    <col min="32" max="34" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="2.88671875" customWidth="1"/>
+    <col min="36" max="36" width="7.21875" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="6.5546875" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="6" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="12.77734375" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="8.5546875" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="8" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="7" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="7.21875" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="45" max="45" width="7.77734375" hidden="1" customWidth="1"/>
+    <col min="46" max="46" width="8.109375" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="13.77734375" customWidth="1"/>
     <col min="48" max="48" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8385,7 +8412,7 @@
         <v>16.07</v>
       </c>
     </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>159</v>
       </c>
@@ -8461,8 +8488,29 @@
       <c r="Y35">
         <v>21.53</v>
       </c>
-    </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU35" s="8">
+        <v>58.02</v>
+      </c>
+      <c r="AV35" s="9">
+        <v>24</v>
+      </c>
+      <c r="AW35" s="1">
+        <v>61.21</v>
+      </c>
+      <c r="AX35" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="AY35" s="2">
+        <v>67.16</v>
+      </c>
+      <c r="AZ35" s="2">
+        <v>61.76</v>
+      </c>
+      <c r="BA35" s="3">
+        <v>22.89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>161</v>
       </c>
@@ -8559,8 +8607,29 @@
       <c r="AF36">
         <v>10.79</v>
       </c>
-    </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU36" s="6">
+        <v>54.7</v>
+      </c>
+      <c r="AV36" s="7">
+        <v>37</v>
+      </c>
+      <c r="AW36" s="1">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="AX36" s="2">
+        <v>53.82</v>
+      </c>
+      <c r="AY36" s="2">
+        <v>57.01</v>
+      </c>
+      <c r="AZ36" s="2">
+        <v>42.37</v>
+      </c>
+      <c r="BA36" s="3">
+        <v>16.43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>164</v>
       </c>
@@ -8678,8 +8747,29 @@
       <c r="AM37">
         <v>22.64</v>
       </c>
-    </row>
-    <row r="38" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU37" s="6">
+        <v>55.65</v>
+      </c>
+      <c r="AV37" s="7">
+        <v>35</v>
+      </c>
+      <c r="AW37" s="1">
+        <v>68.98</v>
+      </c>
+      <c r="AX37" s="2">
+        <v>34.76</v>
+      </c>
+      <c r="AY37" s="2">
+        <v>73.36</v>
+      </c>
+      <c r="AZ37" s="2">
+        <v>56.15</v>
+      </c>
+      <c r="BA37" s="3">
+        <v>42.38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>166</v>
       </c>
@@ -8797,8 +8887,29 @@
       <c r="AT38">
         <v>41</v>
       </c>
-    </row>
-    <row r="39" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU38" s="6">
+        <v>51.69</v>
+      </c>
+      <c r="AV38" s="7">
+        <v>46</v>
+      </c>
+      <c r="AW38" s="1">
+        <v>62.59</v>
+      </c>
+      <c r="AX38" s="2">
+        <v>46.35</v>
+      </c>
+      <c r="AY38" s="2">
+        <v>62.2</v>
+      </c>
+      <c r="AZ38" s="2">
+        <v>55.14</v>
+      </c>
+      <c r="BA38" s="3">
+        <v>10.53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>169</v>
       </c>
@@ -8916,8 +9027,29 @@
       <c r="AT39">
         <v>51</v>
       </c>
-    </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU39" s="6">
+        <v>53.36</v>
+      </c>
+      <c r="AV39" s="7">
+        <v>41</v>
+      </c>
+      <c r="AW39" s="1">
+        <v>70.010000000000005</v>
+      </c>
+      <c r="AX39" s="2">
+        <v>40.17</v>
+      </c>
+      <c r="AY39" s="2">
+        <v>67.290000000000006</v>
+      </c>
+      <c r="AZ39" s="2">
+        <v>55.94</v>
+      </c>
+      <c r="BA39" s="3">
+        <v>12.59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>173</v>
       </c>
@@ -9056,8 +9188,29 @@
       <c r="AT40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU40" s="6">
+        <v>53.06</v>
+      </c>
+      <c r="AV40" s="7">
+        <v>42</v>
+      </c>
+      <c r="AW40" s="1">
+        <v>70.27</v>
+      </c>
+      <c r="AX40" s="2">
+        <v>35.74</v>
+      </c>
+      <c r="AY40" s="2">
+        <v>58.52</v>
+      </c>
+      <c r="AZ40" s="2">
+        <v>76.97</v>
+      </c>
+      <c r="BA40" s="3">
+        <v>18.579999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>175</v>
       </c>
@@ -9175,8 +9328,29 @@
       <c r="AM41">
         <v>27.33</v>
       </c>
-    </row>
-    <row r="42" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU41" s="6">
+        <v>52.37</v>
+      </c>
+      <c r="AV41" s="7">
+        <v>43</v>
+      </c>
+      <c r="AW41" s="1">
+        <v>75.78</v>
+      </c>
+      <c r="AX41" s="2">
+        <v>25.35</v>
+      </c>
+      <c r="AY41" s="2">
+        <v>62.6</v>
+      </c>
+      <c r="AZ41" s="2">
+        <v>61.97</v>
+      </c>
+      <c r="BA41" s="3">
+        <v>33.15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>178</v>
       </c>
@@ -9315,8 +9489,29 @@
       <c r="AT42">
         <v>43</v>
       </c>
-    </row>
-    <row r="43" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU42" s="6">
+        <v>60.43</v>
+      </c>
+      <c r="AV42" s="7">
+        <v>20</v>
+      </c>
+      <c r="AW42" s="1">
+        <v>75.760000000000005</v>
+      </c>
+      <c r="AX42" s="2">
+        <v>44.05</v>
+      </c>
+      <c r="AY42" s="2">
+        <v>77.55</v>
+      </c>
+      <c r="AZ42" s="2">
+        <v>67.16</v>
+      </c>
+      <c r="BA42" s="3">
+        <v>22.57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>183</v>
       </c>
@@ -9455,8 +9650,29 @@
       <c r="AT43">
         <v>82</v>
       </c>
-    </row>
-    <row r="44" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU43" s="6">
+        <v>51.17</v>
+      </c>
+      <c r="AV43" s="7">
+        <v>47</v>
+      </c>
+      <c r="AW43" s="1">
+        <v>59.01</v>
+      </c>
+      <c r="AX43" s="2">
+        <v>37.99</v>
+      </c>
+      <c r="AY43" s="2">
+        <v>75.22</v>
+      </c>
+      <c r="AZ43" s="2">
+        <v>52.15</v>
+      </c>
+      <c r="BA43" s="3">
+        <v>18.23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>186</v>
       </c>
@@ -9595,8 +9811,29 @@
       <c r="AT44">
         <v>86</v>
       </c>
-    </row>
-    <row r="45" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU44" s="6">
+        <v>56.7</v>
+      </c>
+      <c r="AV44" s="7">
+        <v>30</v>
+      </c>
+      <c r="AW44" s="1">
+        <v>78.42</v>
+      </c>
+      <c r="AX44" s="2">
+        <v>34.92</v>
+      </c>
+      <c r="AY44" s="2">
+        <v>74.41</v>
+      </c>
+      <c r="AZ44" s="2">
+        <v>66.44</v>
+      </c>
+      <c r="BA44" s="3">
+        <v>11.78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>189</v>
       </c>
@@ -9735,8 +9972,29 @@
       <c r="AT45">
         <v>41</v>
       </c>
-    </row>
-    <row r="46" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU45">
+        <v>50.11</v>
+      </c>
+      <c r="AV45" s="9">
+        <v>50</v>
+      </c>
+      <c r="AW45" s="1">
+        <v>57.73</v>
+      </c>
+      <c r="AX45" s="2">
+        <v>43.66</v>
+      </c>
+      <c r="AY45" s="2">
+        <v>63.35</v>
+      </c>
+      <c r="AZ45" s="2">
+        <v>55.32</v>
+      </c>
+      <c r="BA45" s="3">
+        <v>14.94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>193</v>
       </c>
@@ -9833,8 +10091,29 @@
       <c r="AF46">
         <v>19.350000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU46" s="6">
+        <v>50.5</v>
+      </c>
+      <c r="AV46" s="7">
+        <v>48</v>
+      </c>
+      <c r="AW46" s="1">
+        <v>63.78</v>
+      </c>
+      <c r="AX46" s="2">
+        <v>37.31</v>
+      </c>
+      <c r="AY46" s="2">
+        <v>63.41</v>
+      </c>
+      <c r="AZ46" s="2">
+        <v>52.63</v>
+      </c>
+      <c r="BA46" s="3">
+        <v>22.25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>196</v>
       </c>
@@ -9973,8 +10252,29 @@
       <c r="AT47">
         <v>90</v>
       </c>
-    </row>
-    <row r="48" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU47" s="6">
+        <v>49.33</v>
+      </c>
+      <c r="AV47" s="7">
+        <v>53</v>
+      </c>
+      <c r="AW47" s="1">
+        <v>66.55</v>
+      </c>
+      <c r="AX47" s="2">
+        <v>34.54</v>
+      </c>
+      <c r="AY47" s="2">
+        <v>56.6</v>
+      </c>
+      <c r="AZ47" s="2">
+        <v>50.59</v>
+      </c>
+      <c r="BA47" s="3">
+        <v>26.21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>199</v>
       </c>
@@ -10113,8 +10413,29 @@
       <c r="AT48">
         <v>83</v>
       </c>
-    </row>
-    <row r="49" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU48" s="6">
+        <v>47.61</v>
+      </c>
+      <c r="AV48" s="7">
+        <v>58</v>
+      </c>
+      <c r="AW48" s="1">
+        <v>56.53</v>
+      </c>
+      <c r="AX48" s="2">
+        <v>38.64</v>
+      </c>
+      <c r="AY48" s="2">
+        <v>65.08</v>
+      </c>
+      <c r="AZ48" s="2">
+        <v>49.87</v>
+      </c>
+      <c r="BA48" s="3">
+        <v>10.53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>202</v>
       </c>
@@ -10253,8 +10574,29 @@
       <c r="AT49">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU49" s="6">
+        <v>54.63</v>
+      </c>
+      <c r="AV49" s="7">
+        <v>38</v>
+      </c>
+      <c r="AW49" s="1">
+        <v>65.489999999999995</v>
+      </c>
+      <c r="AX49" s="2">
+        <v>48</v>
+      </c>
+      <c r="AY49" s="2">
+        <v>66.790000000000006</v>
+      </c>
+      <c r="AZ49" s="2">
+        <v>57.58</v>
+      </c>
+      <c r="BA49" s="3">
+        <v>14.56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>205</v>
       </c>
@@ -10372,8 +10714,29 @@
       <c r="AT50">
         <v>25</v>
       </c>
-    </row>
-    <row r="51" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU50" s="6">
+        <v>49.45</v>
+      </c>
+      <c r="AV50" s="7">
+        <v>52</v>
+      </c>
+      <c r="AW50" s="1">
+        <v>68.14</v>
+      </c>
+      <c r="AX50" s="2">
+        <v>31.7</v>
+      </c>
+      <c r="AY50" s="2">
+        <v>59.18</v>
+      </c>
+      <c r="AZ50" s="2">
+        <v>63.99</v>
+      </c>
+      <c r="BA50" s="3">
+        <v>12.59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>208</v>
       </c>
@@ -10512,8 +10875,29 @@
       <c r="AT51">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU51" s="6">
+        <v>51.93</v>
+      </c>
+      <c r="AV51" s="7">
+        <v>44</v>
+      </c>
+      <c r="AW51" s="1">
+        <v>70.08</v>
+      </c>
+      <c r="AX51" s="2">
+        <v>44.8</v>
+      </c>
+      <c r="AY51" s="2">
+        <v>52.73</v>
+      </c>
+      <c r="AZ51" s="2">
+        <v>56.18</v>
+      </c>
+      <c r="BA51" s="3">
+        <v>12.99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>212</v>
       </c>
@@ -10652,8 +11036,29 @@
       <c r="AT52">
         <v>33</v>
       </c>
-    </row>
-    <row r="53" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU52" s="6">
+        <v>48.33</v>
+      </c>
+      <c r="AV52" s="7">
+        <v>55</v>
+      </c>
+      <c r="AW52" s="1">
+        <v>67.36</v>
+      </c>
+      <c r="AX52" s="2">
+        <v>33.36</v>
+      </c>
+      <c r="AY52" s="2">
+        <v>49.48</v>
+      </c>
+      <c r="AZ52" s="2">
+        <v>62.47</v>
+      </c>
+      <c r="BA52" s="3">
+        <v>19.61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>215</v>
       </c>
@@ -10792,8 +11197,29 @@
       <c r="AT53">
         <v>95</v>
       </c>
-    </row>
-    <row r="54" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU53">
+        <v>44.38</v>
+      </c>
+      <c r="AV53" s="9">
+        <v>72</v>
+      </c>
+      <c r="AW53" s="1">
+        <v>62.33</v>
+      </c>
+      <c r="AX53" s="2">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="AY53" s="2">
+        <v>65.13</v>
+      </c>
+      <c r="AZ53" s="2">
+        <v>51.65</v>
+      </c>
+      <c r="BA53" s="3">
+        <v>23.51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>218</v>
       </c>
@@ -10932,8 +11358,29 @@
       <c r="AT54">
         <v>94</v>
       </c>
-    </row>
-    <row r="55" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU54" s="6">
+        <v>47.68</v>
+      </c>
+      <c r="AV54" s="7">
+        <v>57</v>
+      </c>
+      <c r="AW54" s="1">
+        <v>66.5</v>
+      </c>
+      <c r="AX54" s="2">
+        <v>24.91</v>
+      </c>
+      <c r="AY54" s="2">
+        <v>50.8</v>
+      </c>
+      <c r="AZ54" s="2">
+        <v>48.09</v>
+      </c>
+      <c r="BA54" s="3">
+        <v>52.94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>220</v>
       </c>
@@ -11009,8 +11456,29 @@
       <c r="Y55">
         <v>26.21</v>
       </c>
-    </row>
-    <row r="56" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU55" s="6">
+        <v>46.41</v>
+      </c>
+      <c r="AV55" s="7">
+        <v>62</v>
+      </c>
+      <c r="AW55" s="1">
+        <v>49.16</v>
+      </c>
+      <c r="AX55" s="2">
+        <v>38.57</v>
+      </c>
+      <c r="AY55" s="2">
+        <v>63.99</v>
+      </c>
+      <c r="AZ55" s="2">
+        <v>51.02</v>
+      </c>
+      <c r="BA55" s="3">
+        <v>21.93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>222</v>
       </c>
@@ -11107,8 +11575,29 @@
       <c r="AF56">
         <v>5.04</v>
       </c>
-    </row>
-    <row r="57" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AU56" s="6">
+        <v>48.56</v>
+      </c>
+      <c r="AV56" s="7">
+        <v>54</v>
+      </c>
+      <c r="AW56" s="1">
+        <v>64.87</v>
+      </c>
+      <c r="AX56" s="2">
+        <v>37.36</v>
+      </c>
+      <c r="AY56" s="2">
+        <v>46.78</v>
+      </c>
+      <c r="AZ56" s="2">
+        <v>63.38</v>
+      </c>
+      <c r="BA56" s="3">
+        <v>21.93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>224</v>
       </c>
@@ -11206,7 +11695,7 @@
         <v>3.09</v>
       </c>
     </row>
-    <row r="58" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>227</v>
       </c>
@@ -11262,7 +11751,7 @@
         <v>6.18</v>
       </c>
     </row>
-    <row r="59" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>230</v>
       </c>
@@ -11360,7 +11849,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="60" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>232</v>
       </c>
@@ -11500,7 +11989,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>236</v>
       </c>
@@ -11619,7 +12108,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="62" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>239</v>
       </c>
@@ -11696,7 +12185,7 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="63" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>242</v>
       </c>
@@ -11815,7 +12304,7 @@
         <v>4.82</v>
       </c>
     </row>
-    <row r="64" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>244</v>
       </c>

</xml_diff>